<commit_message>
We optimized so much we have space for fancy GUI in the exe player. this is revision 2024 entry, RC1
</commit_message>
<xml_diff>
--- a/compression20240327.xlsx
+++ b/compression20240327.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\root\git\thenfour\WaveSabre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE28A263-22A0-4380-A7DD-B045D2FD0122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A51A5C-49CD-4BFA-868A-8ED6E74E4977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25490" yWindow="-2490" windowWidth="25820" windowHeight="14020" xr2:uid="{1D2B4EEC-AD31-4B93-9EB2-98EAD4EC652F}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="31">
   <si>
     <t>delta-from-defaults</t>
   </si>
@@ -114,6 +114,12 @@
   <si>
     <t>order by
 worst compr</t>
+  </si>
+  <si>
+    <t>delta16sign</t>
+  </si>
+  <si>
+    <t>ok the awful results earlier wsa from not handling the sign correctly.</t>
   </si>
 </sst>
 </file>
@@ -488,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B1877DF-BC44-423C-9F24-D4095931E820}">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D12" sqref="D2:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,14 +513,15 @@
     <col min="9" max="9" width="14.140625" style="1" customWidth="1"/>
     <col min="10" max="10" width="12.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="85.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="85.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
@@ -549,22 +556,25 @@
         <v>19</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>12883</v>
       </c>
@@ -578,11 +588,11 @@
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>12887</v>
       </c>
@@ -599,11 +609,11 @@
       <c r="J3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>12908</v>
       </c>
@@ -617,17 +627,17 @@
       <c r="F4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>12916</v>
+        <v>12909</v>
       </c>
       <c r="B5">
         <f>A5-13052</f>
-        <v>-136</v>
+        <v>-143</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>4</v>
@@ -635,196 +645,289 @@
       <c r="E5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>12934</v>
+        <v>12911</v>
       </c>
       <c r="B6">
         <f>A6-13052</f>
-        <v>-118</v>
+        <v>-141</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>13043</v>
+        <v>12916</v>
       </c>
       <c r="B7">
         <f>A7-13052</f>
-        <v>-9</v>
+        <v>-136</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>13052</v>
+        <v>12920</v>
       </c>
       <c r="B8">
         <f>A8-13052</f>
-        <v>0</v>
+        <v>-132</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>13086</v>
+        <v>12934</v>
       </c>
       <c r="B9">
         <f>A9-13052</f>
-        <v>34</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+        <v>-118</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>13127</v>
+        <v>13043</v>
       </c>
       <c r="B10">
         <f>A10-13052</f>
-        <v>75</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+        <v>-9</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>13231</v>
+        <v>13052</v>
       </c>
       <c r="B11">
         <f>A11-13052</f>
-        <v>179</v>
-      </c>
-      <c r="P11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>13241</v>
+        <v>13078</v>
       </c>
       <c r="B12">
         <f>A12-13052</f>
+        <v>26</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>13086</v>
+      </c>
+      <c r="B13">
+        <f>A13-13052</f>
+        <v>34</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13093</v>
+      </c>
+      <c r="B14">
+        <f>A14-13052</f>
+        <v>41</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13120</v>
+      </c>
+      <c r="B15">
+        <f>A15-13052</f>
+        <v>68</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>13127</v>
+      </c>
+      <c r="B16">
+        <f>A16-13052</f>
+        <v>75</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>13231</v>
+      </c>
+      <c r="B17">
+        <f>A17-13052</f>
+        <v>179</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>13241</v>
+      </c>
+      <c r="B18">
+        <f>A18-13052</f>
         <v>189</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P12" t="s">
+      <c r="G18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19">
         <f>14000</f>
         <v>14000</v>
       </c>
-      <c r="B13">
-        <f>A13-13052</f>
+      <c r="B19">
+        <f>A19-13052</f>
         <v>948</v>
       </c>
-      <c r="C13">
+      <c r="C19">
         <v>36639</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P13" t="s">
+      <c r="E19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q19" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20">
         <f>14000</f>
         <v>14000</v>
       </c>
-      <c r="B14">
-        <f>A14-13052</f>
+      <c r="B20">
+        <f>A20-13052</f>
         <v>948</v>
       </c>
-      <c r="C14">
+      <c r="C20">
         <v>32753</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P14" t="s">
+      <c r="E20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q20" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21">
         <f>14000</f>
         <v>14000</v>
       </c>
-      <c r="B15">
-        <f>A15-13052</f>
+      <c r="B21">
+        <f>A21-13052</f>
         <v>948</v>
       </c>
-      <c r="C15">
+      <c r="C21">
         <v>26499</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P15" t="s">
+      <c r="E21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>13078</v>
-      </c>
-      <c r="B16">
-        <f>A16-13052</f>
-        <v>26</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P15">
-    <sortCondition ref="A2:A15"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q21">
+    <sortCondition ref="B10:B21"/>
   </sortState>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="dataBar" priority="1">

</xml_diff>